<commit_message>
draw line figures for different training sizes
</commit_message>
<xml_diff>
--- a/Experiment results/CNNs results for world map detection.xlsx
+++ b/Experiment results/CNNs results for world map detection.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\li.7957\Desktop\Map_Identification_Classification\Experiment results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiali\Desktop\Map_Identification_Classification\Experiment results\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5AE07C-4ED5-48FE-910F-990E06484315}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7425"/>
+    <workbookView minimized="1" xWindow="317" yWindow="2169" windowWidth="16457" windowHeight="8520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="28">
   <si>
     <t>Training loss</t>
   </si>
@@ -238,7 +239,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -296,12 +297,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -669,7 +670,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -677,6 +677,360 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>CNNs' Testing Accuracy with different training size</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$198</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Testing accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$199:$A$203</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$199:$B$203</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.49330000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93330000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3501-4071-90FE-8B41965E0305}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="583815792"/>
+        <c:axId val="581148976"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="583815792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="581148976"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="581148976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="583815792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -751,6 +1105,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -901,6 +1295,522 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1287,6 +2197,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>316965</xdr:colOff>
+      <xdr:row>187</xdr:row>
+      <xdr:rowOff>110778</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2321218</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>68515</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D37D9235-074E-4F02-ACCE-7E2062859B9E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1557,21 +2503,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G192" sqref="G192:H203"/>
+    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I191" sqref="I191"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="8" max="8" width="52.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.53515625" customWidth="1"/>
+    <col min="2" max="2" width="16.15234375" customWidth="1"/>
+    <col min="3" max="3" width="20.15234375" customWidth="1"/>
+    <col min="4" max="4" width="20.69140625" customWidth="1"/>
+    <col min="5" max="5" width="17.84375" customWidth="1"/>
+    <col min="8" max="8" width="52.53515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1587,10 +2533,10 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="8"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2">
@@ -1602,61 +2548,61 @@
       <c r="E2">
         <v>0.93600000000000005</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8">
       <c r="B4" s="1"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8">
       <c r="B5" s="1"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8">
       <c r="B6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8">
       <c r="B7" s="1"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8">
       <c r="B8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8">
       <c r="B9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8">
       <c r="B13" s="2"/>
@@ -1693,7 +2639,7 @@
       <c r="E16">
         <v>0.93333330000000003</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="8" t="s">
         <v>6</v>
       </c>
       <c r="H16" s="9"/>
@@ -1772,7 +2718,7 @@
       <c r="E29">
         <v>0.94</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="G29" s="8" t="s">
         <v>23</v>
       </c>
       <c r="H29" s="9"/>
@@ -1857,7 +2803,7 @@
       <c r="E42">
         <v>0.92666666746139503</v>
       </c>
-      <c r="G42" s="6" t="s">
+      <c r="G42" s="8" t="s">
         <v>9</v>
       </c>
       <c r="H42" s="9"/>
@@ -1934,10 +2880,10 @@
       <c r="E57" t="s">
         <v>3</v>
       </c>
-      <c r="G57" s="6" t="s">
+      <c r="G57" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H57" s="6"/>
+      <c r="H57" s="8"/>
     </row>
     <row r="58" spans="1:8">
       <c r="A58">
@@ -1949,57 +2895,57 @@
       <c r="E58">
         <v>0.94000000079472801</v>
       </c>
-      <c r="G58" s="6"/>
-      <c r="H58" s="6"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
     </row>
     <row r="59" spans="1:8">
       <c r="B59" s="1"/>
-      <c r="G59" s="6"/>
-      <c r="H59" s="6"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8"/>
     </row>
     <row r="60" spans="1:8">
-      <c r="G60" s="6"/>
-      <c r="H60" s="6"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
     </row>
     <row r="61" spans="1:8">
       <c r="B61" s="1"/>
-      <c r="G61" s="6"/>
-      <c r="H61" s="6"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8"/>
     </row>
     <row r="62" spans="1:8">
-      <c r="G62" s="6"/>
-      <c r="H62" s="6"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8"/>
     </row>
     <row r="63" spans="1:8">
-      <c r="G63" s="6"/>
-      <c r="H63" s="6"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
     </row>
     <row r="64" spans="1:8">
-      <c r="G64" s="6"/>
-      <c r="H64" s="6"/>
+      <c r="G64" s="8"/>
+      <c r="H64" s="8"/>
     </row>
     <row r="65" spans="1:8">
       <c r="B65" s="1"/>
-      <c r="G65" s="6"/>
-      <c r="H65" s="6"/>
+      <c r="G65" s="8"/>
+      <c r="H65" s="8"/>
     </row>
     <row r="66" spans="1:8">
       <c r="B66" s="1"/>
-      <c r="G66" s="6"/>
-      <c r="H66" s="6"/>
+      <c r="G66" s="8"/>
+      <c r="H66" s="8"/>
     </row>
     <row r="67" spans="1:8">
       <c r="B67" s="1"/>
-      <c r="G67" s="6"/>
-      <c r="H67" s="6"/>
+      <c r="G67" s="8"/>
+      <c r="H67" s="8"/>
     </row>
     <row r="68" spans="1:8">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
-      <c r="G68" s="6"/>
-      <c r="H68" s="6"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
     </row>
     <row r="69" spans="1:8">
       <c r="B69" s="2"/>
@@ -2032,10 +2978,10 @@
       <c r="E70" t="s">
         <v>3</v>
       </c>
-      <c r="G70" s="6" t="s">
+      <c r="G70" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H70" s="6"/>
+      <c r="H70" s="8"/>
     </row>
     <row r="71" spans="1:8">
       <c r="A71">
@@ -2047,53 +2993,53 @@
       <c r="E71">
         <v>0.95000000079472802</v>
       </c>
-      <c r="G71" s="6"/>
-      <c r="H71" s="6"/>
+      <c r="G71" s="8"/>
+      <c r="H71" s="8"/>
     </row>
     <row r="72" spans="1:8">
-      <c r="G72" s="6"/>
-      <c r="H72" s="6"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8"/>
     </row>
     <row r="73" spans="1:8">
-      <c r="G73" s="6"/>
-      <c r="H73" s="6"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="8"/>
     </row>
     <row r="74" spans="1:8">
-      <c r="G74" s="6"/>
-      <c r="H74" s="6"/>
+      <c r="G74" s="8"/>
+      <c r="H74" s="8"/>
     </row>
     <row r="75" spans="1:8">
-      <c r="G75" s="6"/>
-      <c r="H75" s="6"/>
+      <c r="G75" s="8"/>
+      <c r="H75" s="8"/>
     </row>
     <row r="76" spans="1:8">
       <c r="B76" s="1"/>
-      <c r="G76" s="6"/>
-      <c r="H76" s="6"/>
+      <c r="G76" s="8"/>
+      <c r="H76" s="8"/>
     </row>
     <row r="77" spans="1:8">
-      <c r="G77" s="6"/>
-      <c r="H77" s="6"/>
+      <c r="G77" s="8"/>
+      <c r="H77" s="8"/>
     </row>
     <row r="78" spans="1:8">
-      <c r="G78" s="6"/>
-      <c r="H78" s="6"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="8"/>
     </row>
     <row r="79" spans="1:8">
-      <c r="G79" s="6"/>
-      <c r="H79" s="6"/>
+      <c r="G79" s="8"/>
+      <c r="H79" s="8"/>
     </row>
     <row r="80" spans="1:8">
-      <c r="G80" s="6"/>
-      <c r="H80" s="6"/>
+      <c r="G80" s="8"/>
+      <c r="H80" s="8"/>
     </row>
     <row r="81" spans="1:8">
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
-      <c r="G81" s="6"/>
-      <c r="H81" s="6"/>
+      <c r="G81" s="8"/>
+      <c r="H81" s="8"/>
     </row>
     <row r="82" spans="1:8">
       <c r="B82" s="2"/>
@@ -2127,10 +3073,10 @@
       <c r="E84" t="s">
         <v>3</v>
       </c>
-      <c r="G84" s="6" t="s">
+      <c r="G84" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H84" s="6"/>
+      <c r="H84" s="8"/>
     </row>
     <row r="85" spans="1:8">
       <c r="A85">
@@ -2143,61 +3089,61 @@
       <c r="E85">
         <v>0.94</v>
       </c>
-      <c r="G85" s="6"/>
-      <c r="H85" s="6"/>
+      <c r="G85" s="8"/>
+      <c r="H85" s="8"/>
     </row>
     <row r="86" spans="1:8">
       <c r="B86" s="1"/>
-      <c r="G86" s="6"/>
-      <c r="H86" s="6"/>
+      <c r="G86" s="8"/>
+      <c r="H86" s="8"/>
     </row>
     <row r="87" spans="1:8">
       <c r="B87" s="1"/>
-      <c r="G87" s="6"/>
-      <c r="H87" s="6"/>
+      <c r="G87" s="8"/>
+      <c r="H87" s="8"/>
     </row>
     <row r="88" spans="1:8">
       <c r="B88" s="1"/>
-      <c r="G88" s="6"/>
-      <c r="H88" s="6"/>
+      <c r="G88" s="8"/>
+      <c r="H88" s="8"/>
     </row>
     <row r="89" spans="1:8">
       <c r="B89" s="1"/>
-      <c r="G89" s="6"/>
-      <c r="H89" s="6"/>
+      <c r="G89" s="8"/>
+      <c r="H89" s="8"/>
     </row>
     <row r="90" spans="1:8">
       <c r="B90" s="1"/>
-      <c r="G90" s="6"/>
-      <c r="H90" s="6"/>
+      <c r="G90" s="8"/>
+      <c r="H90" s="8"/>
     </row>
     <row r="91" spans="1:8">
       <c r="B91" s="1"/>
-      <c r="G91" s="6"/>
-      <c r="H91" s="6"/>
+      <c r="G91" s="8"/>
+      <c r="H91" s="8"/>
     </row>
     <row r="92" spans="1:8">
       <c r="B92" s="1"/>
-      <c r="G92" s="6"/>
-      <c r="H92" s="6"/>
+      <c r="G92" s="8"/>
+      <c r="H92" s="8"/>
     </row>
     <row r="93" spans="1:8">
       <c r="B93" s="1"/>
-      <c r="G93" s="6"/>
-      <c r="H93" s="6"/>
+      <c r="G93" s="8"/>
+      <c r="H93" s="8"/>
     </row>
     <row r="94" spans="1:8">
       <c r="B94" s="1"/>
-      <c r="G94" s="6"/>
-      <c r="H94" s="6"/>
+      <c r="G94" s="8"/>
+      <c r="H94" s="8"/>
     </row>
     <row r="95" spans="1:8">
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
-      <c r="G95" s="6"/>
-      <c r="H95" s="6"/>
+      <c r="G95" s="8"/>
+      <c r="H95" s="8"/>
     </row>
     <row r="96" spans="1:8">
       <c r="B96" s="2"/>
@@ -2223,10 +3169,10 @@
       <c r="E97" t="s">
         <v>3</v>
       </c>
-      <c r="G97" s="6" t="s">
+      <c r="G97" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H97" s="6"/>
+      <c r="H97" s="8"/>
     </row>
     <row r="98" spans="1:8">
       <c r="A98">
@@ -2238,52 +3184,52 @@
       <c r="E98">
         <v>0.94333333412806197</v>
       </c>
-      <c r="G98" s="6"/>
-      <c r="H98" s="6"/>
+      <c r="G98" s="8"/>
+      <c r="H98" s="8"/>
     </row>
     <row r="99" spans="1:8">
-      <c r="G99" s="6"/>
-      <c r="H99" s="6"/>
+      <c r="G99" s="8"/>
+      <c r="H99" s="8"/>
     </row>
     <row r="100" spans="1:8">
-      <c r="G100" s="6"/>
-      <c r="H100" s="6"/>
+      <c r="G100" s="8"/>
+      <c r="H100" s="8"/>
     </row>
     <row r="101" spans="1:8">
-      <c r="G101" s="6"/>
-      <c r="H101" s="6"/>
+      <c r="G101" s="8"/>
+      <c r="H101" s="8"/>
     </row>
     <row r="102" spans="1:8">
-      <c r="G102" s="6"/>
-      <c r="H102" s="6"/>
+      <c r="G102" s="8"/>
+      <c r="H102" s="8"/>
     </row>
     <row r="103" spans="1:8">
-      <c r="G103" s="6"/>
-      <c r="H103" s="6"/>
+      <c r="G103" s="8"/>
+      <c r="H103" s="8"/>
     </row>
     <row r="104" spans="1:8">
-      <c r="G104" s="6"/>
-      <c r="H104" s="6"/>
+      <c r="G104" s="8"/>
+      <c r="H104" s="8"/>
     </row>
     <row r="105" spans="1:8">
-      <c r="G105" s="6"/>
-      <c r="H105" s="6"/>
+      <c r="G105" s="8"/>
+      <c r="H105" s="8"/>
     </row>
     <row r="106" spans="1:8">
-      <c r="G106" s="6"/>
-      <c r="H106" s="6"/>
+      <c r="G106" s="8"/>
+      <c r="H106" s="8"/>
     </row>
     <row r="107" spans="1:8">
-      <c r="G107" s="6"/>
-      <c r="H107" s="6"/>
+      <c r="G107" s="8"/>
+      <c r="H107" s="8"/>
     </row>
     <row r="108" spans="1:8">
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
-      <c r="G108" s="6"/>
-      <c r="H108" s="6"/>
+      <c r="G108" s="8"/>
+      <c r="H108" s="8"/>
     </row>
     <row r="109" spans="1:8">
       <c r="B109" s="2"/>
@@ -2309,10 +3255,10 @@
       <c r="E110" t="s">
         <v>3</v>
       </c>
-      <c r="G110" s="6" t="s">
+      <c r="G110" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H110" s="6"/>
+      <c r="H110" s="8"/>
     </row>
     <row r="111" spans="1:8">
       <c r="A111">
@@ -2324,52 +3270,52 @@
       <c r="E111">
         <v>0.94333333333333302</v>
       </c>
-      <c r="G111" s="6"/>
-      <c r="H111" s="6"/>
+      <c r="G111" s="8"/>
+      <c r="H111" s="8"/>
     </row>
     <row r="112" spans="1:8">
-      <c r="G112" s="6"/>
-      <c r="H112" s="6"/>
+      <c r="G112" s="8"/>
+      <c r="H112" s="8"/>
     </row>
     <row r="113" spans="1:8">
-      <c r="G113" s="6"/>
-      <c r="H113" s="6"/>
+      <c r="G113" s="8"/>
+      <c r="H113" s="8"/>
     </row>
     <row r="114" spans="1:8">
-      <c r="G114" s="6"/>
-      <c r="H114" s="6"/>
+      <c r="G114" s="8"/>
+      <c r="H114" s="8"/>
     </row>
     <row r="115" spans="1:8">
-      <c r="G115" s="6"/>
-      <c r="H115" s="6"/>
+      <c r="G115" s="8"/>
+      <c r="H115" s="8"/>
     </row>
     <row r="116" spans="1:8">
-      <c r="G116" s="6"/>
-      <c r="H116" s="6"/>
+      <c r="G116" s="8"/>
+      <c r="H116" s="8"/>
     </row>
     <row r="117" spans="1:8">
-      <c r="G117" s="6"/>
-      <c r="H117" s="6"/>
+      <c r="G117" s="8"/>
+      <c r="H117" s="8"/>
     </row>
     <row r="118" spans="1:8">
-      <c r="G118" s="6"/>
-      <c r="H118" s="6"/>
+      <c r="G118" s="8"/>
+      <c r="H118" s="8"/>
     </row>
     <row r="119" spans="1:8">
-      <c r="G119" s="6"/>
-      <c r="H119" s="6"/>
+      <c r="G119" s="8"/>
+      <c r="H119" s="8"/>
     </row>
     <row r="120" spans="1:8">
-      <c r="G120" s="6"/>
-      <c r="H120" s="6"/>
+      <c r="G120" s="8"/>
+      <c r="H120" s="8"/>
     </row>
     <row r="121" spans="1:8">
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
-      <c r="G121" s="6"/>
-      <c r="H121" s="6"/>
+      <c r="G121" s="8"/>
+      <c r="H121" s="8"/>
     </row>
     <row r="122" spans="1:8">
       <c r="B122" s="2"/>
@@ -2419,10 +3365,10 @@
       <c r="E126" t="s">
         <v>3</v>
       </c>
-      <c r="G126" s="6" t="s">
+      <c r="G126" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H126" s="6"/>
+      <c r="H126" s="8"/>
     </row>
     <row r="127" spans="1:8">
       <c r="A127">
@@ -2434,53 +3380,53 @@
       <c r="E127">
         <v>0.49333333333333301</v>
       </c>
-      <c r="G127" s="6"/>
-      <c r="H127" s="6"/>
+      <c r="G127" s="8"/>
+      <c r="H127" s="8"/>
     </row>
     <row r="128" spans="1:8">
-      <c r="G128" s="6"/>
-      <c r="H128" s="6"/>
+      <c r="G128" s="8"/>
+      <c r="H128" s="8"/>
     </row>
     <row r="129" spans="1:8">
-      <c r="G129" s="6"/>
-      <c r="H129" s="6"/>
+      <c r="G129" s="8"/>
+      <c r="H129" s="8"/>
     </row>
     <row r="130" spans="1:8">
-      <c r="G130" s="6"/>
-      <c r="H130" s="6"/>
+      <c r="G130" s="8"/>
+      <c r="H130" s="8"/>
     </row>
     <row r="131" spans="1:8">
-      <c r="G131" s="6"/>
-      <c r="H131" s="6"/>
+      <c r="G131" s="8"/>
+      <c r="H131" s="8"/>
     </row>
     <row r="132" spans="1:8">
-      <c r="G132" s="6"/>
-      <c r="H132" s="6"/>
+      <c r="G132" s="8"/>
+      <c r="H132" s="8"/>
     </row>
     <row r="133" spans="1:8">
       <c r="B133" s="1"/>
-      <c r="G133" s="6"/>
-      <c r="H133" s="6"/>
+      <c r="G133" s="8"/>
+      <c r="H133" s="8"/>
     </row>
     <row r="134" spans="1:8">
-      <c r="G134" s="6"/>
-      <c r="H134" s="6"/>
+      <c r="G134" s="8"/>
+      <c r="H134" s="8"/>
     </row>
     <row r="135" spans="1:8">
-      <c r="G135" s="6"/>
-      <c r="H135" s="6"/>
+      <c r="G135" s="8"/>
+      <c r="H135" s="8"/>
     </row>
     <row r="136" spans="1:8">
-      <c r="G136" s="6"/>
-      <c r="H136" s="6"/>
+      <c r="G136" s="8"/>
+      <c r="H136" s="8"/>
     </row>
     <row r="137" spans="1:8">
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
       <c r="D137" s="2"/>
       <c r="E137" s="2"/>
-      <c r="G137" s="6"/>
-      <c r="H137" s="6"/>
+      <c r="G137" s="8"/>
+      <c r="H137" s="8"/>
     </row>
     <row r="138" spans="1:8">
       <c r="B138" s="2"/>
@@ -2504,10 +3450,10 @@
       <c r="E139" t="s">
         <v>3</v>
       </c>
-      <c r="G139" s="6" t="s">
+      <c r="G139" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H139" s="6"/>
+      <c r="H139" s="8"/>
     </row>
     <row r="140" spans="1:8">
       <c r="A140">
@@ -2519,53 +3465,53 @@
       <c r="E140">
         <v>0.94666666587193005</v>
       </c>
-      <c r="G140" s="6"/>
-      <c r="H140" s="6"/>
+      <c r="G140" s="8"/>
+      <c r="H140" s="8"/>
     </row>
     <row r="141" spans="1:8">
-      <c r="G141" s="6"/>
-      <c r="H141" s="6"/>
+      <c r="G141" s="8"/>
+      <c r="H141" s="8"/>
     </row>
     <row r="142" spans="1:8">
-      <c r="G142" s="6"/>
-      <c r="H142" s="6"/>
+      <c r="G142" s="8"/>
+      <c r="H142" s="8"/>
     </row>
     <row r="143" spans="1:8">
-      <c r="G143" s="6"/>
-      <c r="H143" s="6"/>
+      <c r="G143" s="8"/>
+      <c r="H143" s="8"/>
     </row>
     <row r="144" spans="1:8">
-      <c r="G144" s="6"/>
-      <c r="H144" s="6"/>
+      <c r="G144" s="8"/>
+      <c r="H144" s="8"/>
     </row>
     <row r="145" spans="1:8">
-      <c r="G145" s="6"/>
-      <c r="H145" s="6"/>
+      <c r="G145" s="8"/>
+      <c r="H145" s="8"/>
     </row>
     <row r="146" spans="1:8">
       <c r="B146" s="1"/>
-      <c r="G146" s="6"/>
-      <c r="H146" s="6"/>
+      <c r="G146" s="8"/>
+      <c r="H146" s="8"/>
     </row>
     <row r="147" spans="1:8">
-      <c r="G147" s="6"/>
-      <c r="H147" s="6"/>
+      <c r="G147" s="8"/>
+      <c r="H147" s="8"/>
     </row>
     <row r="148" spans="1:8">
-      <c r="G148" s="6"/>
-      <c r="H148" s="6"/>
+      <c r="G148" s="8"/>
+      <c r="H148" s="8"/>
     </row>
     <row r="149" spans="1:8">
-      <c r="G149" s="6"/>
-      <c r="H149" s="6"/>
+      <c r="G149" s="8"/>
+      <c r="H149" s="8"/>
     </row>
     <row r="150" spans="1:8">
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
       <c r="D150" s="2"/>
       <c r="E150" s="2"/>
-      <c r="G150" s="6"/>
-      <c r="H150" s="6"/>
+      <c r="G150" s="8"/>
+      <c r="H150" s="8"/>
     </row>
     <row r="151" spans="1:8">
       <c r="B151" s="2"/>
@@ -2589,10 +3535,10 @@
       <c r="E152" t="s">
         <v>3</v>
       </c>
-      <c r="G152" s="6" t="s">
+      <c r="G152" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H152" s="6"/>
+      <c r="H152" s="8"/>
     </row>
     <row r="153" spans="1:8">
       <c r="A153">
@@ -2604,53 +3550,53 @@
       <c r="E153">
         <v>0.93999999920520005</v>
       </c>
-      <c r="G153" s="6"/>
-      <c r="H153" s="6"/>
+      <c r="G153" s="8"/>
+      <c r="H153" s="8"/>
     </row>
     <row r="154" spans="1:8">
-      <c r="G154" s="6"/>
-      <c r="H154" s="6"/>
+      <c r="G154" s="8"/>
+      <c r="H154" s="8"/>
     </row>
     <row r="155" spans="1:8">
-      <c r="G155" s="6"/>
-      <c r="H155" s="6"/>
+      <c r="G155" s="8"/>
+      <c r="H155" s="8"/>
     </row>
     <row r="156" spans="1:8">
-      <c r="G156" s="6"/>
-      <c r="H156" s="6"/>
+      <c r="G156" s="8"/>
+      <c r="H156" s="8"/>
     </row>
     <row r="157" spans="1:8">
-      <c r="G157" s="6"/>
-      <c r="H157" s="6"/>
+      <c r="G157" s="8"/>
+      <c r="H157" s="8"/>
     </row>
     <row r="158" spans="1:8">
-      <c r="G158" s="6"/>
-      <c r="H158" s="6"/>
+      <c r="G158" s="8"/>
+      <c r="H158" s="8"/>
     </row>
     <row r="159" spans="1:8">
       <c r="B159" s="1"/>
-      <c r="G159" s="6"/>
-      <c r="H159" s="6"/>
+      <c r="G159" s="8"/>
+      <c r="H159" s="8"/>
     </row>
     <row r="160" spans="1:8">
-      <c r="G160" s="6"/>
-      <c r="H160" s="6"/>
+      <c r="G160" s="8"/>
+      <c r="H160" s="8"/>
     </row>
     <row r="161" spans="1:8">
-      <c r="G161" s="6"/>
-      <c r="H161" s="6"/>
+      <c r="G161" s="8"/>
+      <c r="H161" s="8"/>
     </row>
     <row r="162" spans="1:8">
-      <c r="G162" s="6"/>
-      <c r="H162" s="6"/>
+      <c r="G162" s="8"/>
+      <c r="H162" s="8"/>
     </row>
     <row r="163" spans="1:8">
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
       <c r="D163" s="2"/>
       <c r="E163" s="2"/>
-      <c r="G163" s="6"/>
-      <c r="H163" s="6"/>
+      <c r="G163" s="8"/>
+      <c r="H163" s="8"/>
     </row>
     <row r="164" spans="1:8">
       <c r="B164" s="2"/>
@@ -2674,62 +3620,62 @@
       <c r="E165" t="s">
         <v>3</v>
       </c>
-      <c r="G165" s="6" t="s">
+      <c r="G165" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H165" s="6"/>
+      <c r="H165" s="8"/>
     </row>
     <row r="166" spans="1:8">
       <c r="A166">
         <v>1</v>
       </c>
-      <c r="G166" s="6"/>
-      <c r="H166" s="6"/>
+      <c r="G166" s="8"/>
+      <c r="H166" s="8"/>
     </row>
     <row r="167" spans="1:8">
-      <c r="G167" s="6"/>
-      <c r="H167" s="6"/>
+      <c r="G167" s="8"/>
+      <c r="H167" s="8"/>
     </row>
     <row r="168" spans="1:8">
-      <c r="G168" s="6"/>
-      <c r="H168" s="6"/>
+      <c r="G168" s="8"/>
+      <c r="H168" s="8"/>
     </row>
     <row r="169" spans="1:8">
-      <c r="G169" s="6"/>
-      <c r="H169" s="6"/>
+      <c r="G169" s="8"/>
+      <c r="H169" s="8"/>
     </row>
     <row r="170" spans="1:8">
-      <c r="G170" s="6"/>
-      <c r="H170" s="6"/>
+      <c r="G170" s="8"/>
+      <c r="H170" s="8"/>
     </row>
     <row r="171" spans="1:8">
-      <c r="G171" s="6"/>
-      <c r="H171" s="6"/>
+      <c r="G171" s="8"/>
+      <c r="H171" s="8"/>
     </row>
     <row r="172" spans="1:8">
       <c r="B172" s="1"/>
-      <c r="G172" s="6"/>
-      <c r="H172" s="6"/>
+      <c r="G172" s="8"/>
+      <c r="H172" s="8"/>
     </row>
     <row r="173" spans="1:8">
-      <c r="G173" s="6"/>
-      <c r="H173" s="6"/>
+      <c r="G173" s="8"/>
+      <c r="H173" s="8"/>
     </row>
     <row r="174" spans="1:8">
-      <c r="G174" s="6"/>
-      <c r="H174" s="6"/>
+      <c r="G174" s="8"/>
+      <c r="H174" s="8"/>
     </row>
     <row r="175" spans="1:8">
-      <c r="G175" s="6"/>
-      <c r="H175" s="6"/>
+      <c r="G175" s="8"/>
+      <c r="H175" s="8"/>
     </row>
     <row r="176" spans="1:8">
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
       <c r="D176" s="2"/>
       <c r="E176" s="2"/>
-      <c r="G176" s="6"/>
-      <c r="H176" s="6"/>
+      <c r="G176" s="8"/>
+      <c r="H176" s="8"/>
     </row>
     <row r="177" spans="1:8">
       <c r="B177" s="2"/>
@@ -2753,10 +3699,10 @@
       <c r="E178" t="s">
         <v>3</v>
       </c>
-      <c r="G178" s="6" t="s">
+      <c r="G178" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H178" s="6"/>
+      <c r="H178" s="8"/>
     </row>
     <row r="179" spans="1:8">
       <c r="A179">
@@ -2768,53 +3714,53 @@
       <c r="E179">
         <v>0.93333333409999997</v>
       </c>
-      <c r="G179" s="6"/>
-      <c r="H179" s="6"/>
+      <c r="G179" s="8"/>
+      <c r="H179" s="8"/>
     </row>
     <row r="180" spans="1:8">
-      <c r="G180" s="6"/>
-      <c r="H180" s="6"/>
+      <c r="G180" s="8"/>
+      <c r="H180" s="8"/>
     </row>
     <row r="181" spans="1:8">
-      <c r="G181" s="6"/>
-      <c r="H181" s="6"/>
+      <c r="G181" s="8"/>
+      <c r="H181" s="8"/>
     </row>
     <row r="182" spans="1:8">
-      <c r="G182" s="6"/>
-      <c r="H182" s="6"/>
+      <c r="G182" s="8"/>
+      <c r="H182" s="8"/>
     </row>
     <row r="183" spans="1:8">
-      <c r="G183" s="6"/>
-      <c r="H183" s="6"/>
+      <c r="G183" s="8"/>
+      <c r="H183" s="8"/>
     </row>
     <row r="184" spans="1:8">
-      <c r="G184" s="6"/>
-      <c r="H184" s="6"/>
+      <c r="G184" s="8"/>
+      <c r="H184" s="8"/>
     </row>
     <row r="185" spans="1:8">
       <c r="B185" s="1"/>
-      <c r="G185" s="6"/>
-      <c r="H185" s="6"/>
+      <c r="G185" s="8"/>
+      <c r="H185" s="8"/>
     </row>
     <row r="186" spans="1:8">
-      <c r="G186" s="6"/>
-      <c r="H186" s="6"/>
+      <c r="G186" s="8"/>
+      <c r="H186" s="8"/>
     </row>
     <row r="187" spans="1:8">
-      <c r="G187" s="6"/>
-      <c r="H187" s="6"/>
+      <c r="G187" s="8"/>
+      <c r="H187" s="8"/>
     </row>
     <row r="188" spans="1:8">
-      <c r="G188" s="6"/>
-      <c r="H188" s="6"/>
+      <c r="G188" s="8"/>
+      <c r="H188" s="8"/>
     </row>
     <row r="189" spans="1:8">
       <c r="B189" s="2"/>
       <c r="C189" s="2"/>
       <c r="D189" s="2"/>
       <c r="E189" s="2"/>
-      <c r="G189" s="6"/>
-      <c r="H189" s="6"/>
+      <c r="G189" s="8"/>
+      <c r="H189" s="8"/>
     </row>
     <row r="191" spans="1:8">
       <c r="A191" t="s">
@@ -2837,8 +3783,8 @@
       <c r="C192">
         <v>0.95</v>
       </c>
-      <c r="G192" s="6"/>
-      <c r="H192" s="6"/>
+      <c r="G192" s="8"/>
+      <c r="H192" s="8"/>
     </row>
     <row r="193" spans="1:8">
       <c r="A193">
@@ -2850,8 +3796,8 @@
       <c r="C193">
         <v>0.93</v>
       </c>
-      <c r="G193" s="6"/>
-      <c r="H193" s="6"/>
+      <c r="G193" s="8"/>
+      <c r="H193" s="8"/>
     </row>
     <row r="194" spans="1:8">
       <c r="A194">
@@ -2863,8 +3809,8 @@
       <c r="C194">
         <v>0.93330000000000002</v>
       </c>
-      <c r="G194" s="6"/>
-      <c r="H194" s="6"/>
+      <c r="G194" s="8"/>
+      <c r="H194" s="8"/>
     </row>
     <row r="195" spans="1:8">
       <c r="A195">
@@ -2876,8 +3822,8 @@
       <c r="C195">
         <v>0.88</v>
       </c>
-      <c r="G195" s="6"/>
-      <c r="H195" s="6"/>
+      <c r="G195" s="8"/>
+      <c r="H195" s="8"/>
     </row>
     <row r="196" spans="1:8">
       <c r="A196">
@@ -2889,113 +3835,147 @@
       <c r="C196">
         <v>0.49330000000000002</v>
       </c>
-      <c r="G196" s="6"/>
-      <c r="H196" s="6"/>
+      <c r="G196" s="8"/>
+      <c r="H196" s="8"/>
     </row>
     <row r="197" spans="1:8">
-      <c r="G197" s="6"/>
-      <c r="H197" s="6"/>
+      <c r="G197" s="8"/>
+      <c r="H197" s="8"/>
     </row>
     <row r="198" spans="1:8">
-      <c r="G198" s="6"/>
-      <c r="H198" s="6"/>
+      <c r="A198" t="s">
+        <v>26</v>
+      </c>
+      <c r="B198" t="s">
+        <v>27</v>
+      </c>
+      <c r="G198" s="8"/>
+      <c r="H198" s="8"/>
     </row>
     <row r="199" spans="1:8">
-      <c r="B199" s="1"/>
-      <c r="G199" s="6"/>
-      <c r="H199" s="6"/>
+      <c r="A199">
+        <v>300</v>
+      </c>
+      <c r="B199">
+        <v>0.49330000000000002</v>
+      </c>
+      <c r="G199" s="8"/>
+      <c r="H199" s="8"/>
     </row>
     <row r="200" spans="1:8">
-      <c r="G200" s="6"/>
-      <c r="H200" s="6"/>
+      <c r="A200">
+        <v>400</v>
+      </c>
+      <c r="B200">
+        <v>0.88</v>
+      </c>
+      <c r="G200" s="8"/>
+      <c r="H200" s="8"/>
     </row>
     <row r="201" spans="1:8">
-      <c r="G201" s="6"/>
-      <c r="H201" s="6"/>
+      <c r="A201">
+        <v>500</v>
+      </c>
+      <c r="B201">
+        <v>0.93330000000000002</v>
+      </c>
+      <c r="G201" s="8"/>
+      <c r="H201" s="8"/>
     </row>
     <row r="202" spans="1:8">
-      <c r="G202" s="6"/>
-      <c r="H202" s="6"/>
+      <c r="A202">
+        <v>600</v>
+      </c>
+      <c r="B202">
+        <v>0.93</v>
+      </c>
+      <c r="G202" s="8"/>
+      <c r="H202" s="8"/>
     </row>
     <row r="203" spans="1:8">
-      <c r="B203" s="2"/>
+      <c r="A203">
+        <v>700</v>
+      </c>
+      <c r="B203">
+        <v>0.95</v>
+      </c>
       <c r="C203" s="2"/>
       <c r="D203" s="2"/>
       <c r="E203" s="2"/>
-      <c r="G203" s="6"/>
-      <c r="H203" s="6"/>
+      <c r="G203" s="8"/>
+      <c r="H203" s="8"/>
     </row>
     <row r="205" spans="1:8">
-      <c r="G205" s="6"/>
-      <c r="H205" s="6"/>
+      <c r="G205" s="8"/>
+      <c r="H205" s="8"/>
     </row>
     <row r="206" spans="1:8">
-      <c r="G206" s="6"/>
-      <c r="H206" s="6"/>
+      <c r="G206" s="8"/>
+      <c r="H206" s="8"/>
     </row>
     <row r="207" spans="1:8">
-      <c r="G207" s="6"/>
-      <c r="H207" s="6"/>
+      <c r="G207" s="8"/>
+      <c r="H207" s="8"/>
     </row>
     <row r="208" spans="1:8">
-      <c r="G208" s="6"/>
-      <c r="H208" s="6"/>
+      <c r="G208" s="8"/>
+      <c r="H208" s="8"/>
     </row>
     <row r="209" spans="2:8">
-      <c r="G209" s="6"/>
-      <c r="H209" s="6"/>
+      <c r="G209" s="8"/>
+      <c r="H209" s="8"/>
     </row>
     <row r="210" spans="2:8">
-      <c r="G210" s="6"/>
-      <c r="H210" s="6"/>
+      <c r="G210" s="8"/>
+      <c r="H210" s="8"/>
     </row>
     <row r="211" spans="2:8">
-      <c r="G211" s="6"/>
-      <c r="H211" s="6"/>
+      <c r="G211" s="8"/>
+      <c r="H211" s="8"/>
     </row>
     <row r="212" spans="2:8">
       <c r="B212" s="1"/>
-      <c r="G212" s="6"/>
-      <c r="H212" s="6"/>
+      <c r="G212" s="8"/>
+      <c r="H212" s="8"/>
     </row>
     <row r="213" spans="2:8">
-      <c r="G213" s="6"/>
-      <c r="H213" s="6"/>
+      <c r="G213" s="8"/>
+      <c r="H213" s="8"/>
     </row>
     <row r="214" spans="2:8">
-      <c r="G214" s="6"/>
-      <c r="H214" s="6"/>
+      <c r="G214" s="8"/>
+      <c r="H214" s="8"/>
     </row>
     <row r="215" spans="2:8">
-      <c r="G215" s="6"/>
-      <c r="H215" s="6"/>
+      <c r="G215" s="8"/>
+      <c r="H215" s="8"/>
     </row>
     <row r="216" spans="2:8">
       <c r="B216" s="2"/>
       <c r="C216" s="2"/>
       <c r="D216" s="2"/>
       <c r="E216" s="2"/>
-      <c r="G216" s="6"/>
-      <c r="H216" s="6"/>
+      <c r="G216" s="8"/>
+      <c r="H216" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="G1:H12"/>
-    <mergeCell ref="G16:H26"/>
-    <mergeCell ref="G29:H39"/>
-    <mergeCell ref="G42:H52"/>
-    <mergeCell ref="G57:H68"/>
-    <mergeCell ref="G70:H81"/>
-    <mergeCell ref="G84:H95"/>
-    <mergeCell ref="G97:H108"/>
-    <mergeCell ref="G110:H121"/>
-    <mergeCell ref="G126:H137"/>
     <mergeCell ref="G205:H216"/>
     <mergeCell ref="G139:H150"/>
     <mergeCell ref="G152:H163"/>
     <mergeCell ref="G165:H176"/>
     <mergeCell ref="G178:H189"/>
     <mergeCell ref="G192:H203"/>
+    <mergeCell ref="G70:H81"/>
+    <mergeCell ref="G84:H95"/>
+    <mergeCell ref="G97:H108"/>
+    <mergeCell ref="G110:H121"/>
+    <mergeCell ref="G126:H137"/>
+    <mergeCell ref="G1:H12"/>
+    <mergeCell ref="G16:H26"/>
+    <mergeCell ref="G29:H39"/>
+    <mergeCell ref="G42:H52"/>
+    <mergeCell ref="G57:H68"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update CNNs results for world map detection.xlsx
</commit_message>
<xml_diff>
--- a/Experiment results/CNNs results for world map detection.xlsx
+++ b/Experiment results/CNNs results for world map detection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiali\Desktop\Map_Identification_Classification\Experiment results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5AE07C-4ED5-48FE-910F-990E06484315}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF0611D-9E2B-4A0A-AA2F-C867A857719C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="317" yWindow="2169" windowWidth="16457" windowHeight="8520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -240,7 +242,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,13 +266,25 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -282,10 +296,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -297,17 +312,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2205,15 +2224,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>316965</xdr:colOff>
-      <xdr:row>187</xdr:row>
-      <xdr:rowOff>110778</xdr:rowOff>
+      <xdr:colOff>160083</xdr:colOff>
+      <xdr:row>193</xdr:row>
+      <xdr:rowOff>103308</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2321218</xdr:colOff>
-      <xdr:row>202</xdr:row>
-      <xdr:rowOff>68515</xdr:rowOff>
+      <xdr:colOff>2164336</xdr:colOff>
+      <xdr:row>208</xdr:row>
+      <xdr:rowOff>61045</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2506,18 +2525,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I191" sqref="I191"/>
+    <sheetView tabSelected="1" topLeftCell="A169" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G152" sqref="G152:H163"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18.53515625" customWidth="1"/>
-    <col min="2" max="2" width="16.15234375" customWidth="1"/>
-    <col min="3" max="3" width="20.15234375" customWidth="1"/>
-    <col min="4" max="4" width="20.69140625" customWidth="1"/>
-    <col min="5" max="5" width="17.84375" customWidth="1"/>
-    <col min="8" max="8" width="52.53515625" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" customWidth="1"/>
+    <col min="4" max="4" width="20.7265625" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" customWidth="1"/>
+    <col min="8" max="8" width="52.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2533,10 +2552,10 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="7"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2">
@@ -2548,61 +2567,61 @@
       <c r="E2">
         <v>0.93600000000000005</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8">
       <c r="B4" s="1"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8">
       <c r="B5" s="1"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8">
       <c r="B6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:8">
       <c r="B7" s="1"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8">
       <c r="B8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:8">
       <c r="B9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:8">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:8">
       <c r="B13" s="2"/>
@@ -2639,7 +2658,7 @@
       <c r="E16">
         <v>0.93333330000000003</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="6" t="s">
         <v>6</v>
       </c>
       <c r="H16" s="9"/>
@@ -2718,7 +2737,7 @@
       <c r="E29">
         <v>0.94</v>
       </c>
-      <c r="G29" s="8" t="s">
+      <c r="G29" s="6" t="s">
         <v>23</v>
       </c>
       <c r="H29" s="9"/>
@@ -2803,7 +2822,7 @@
       <c r="E42">
         <v>0.92666666746139503</v>
       </c>
-      <c r="G42" s="8" t="s">
+      <c r="G42" s="6" t="s">
         <v>9</v>
       </c>
       <c r="H42" s="9"/>
@@ -2880,10 +2899,10 @@
       <c r="E57" t="s">
         <v>3</v>
       </c>
-      <c r="G57" s="8" t="s">
+      <c r="G57" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H57" s="8"/>
+      <c r="H57" s="6"/>
     </row>
     <row r="58" spans="1:8">
       <c r="A58">
@@ -2895,57 +2914,57 @@
       <c r="E58">
         <v>0.94000000079472801</v>
       </c>
-      <c r="G58" s="8"/>
-      <c r="H58" s="8"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
     </row>
     <row r="59" spans="1:8">
       <c r="B59" s="1"/>
-      <c r="G59" s="8"/>
-      <c r="H59" s="8"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
     </row>
     <row r="60" spans="1:8">
-      <c r="G60" s="8"/>
-      <c r="H60" s="8"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
     </row>
     <row r="61" spans="1:8">
       <c r="B61" s="1"/>
-      <c r="G61" s="8"/>
-      <c r="H61" s="8"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
     </row>
     <row r="62" spans="1:8">
-      <c r="G62" s="8"/>
-      <c r="H62" s="8"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
     </row>
     <row r="63" spans="1:8">
-      <c r="G63" s="8"/>
-      <c r="H63" s="8"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
     </row>
     <row r="64" spans="1:8">
-      <c r="G64" s="8"/>
-      <c r="H64" s="8"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
     </row>
     <row r="65" spans="1:8">
       <c r="B65" s="1"/>
-      <c r="G65" s="8"/>
-      <c r="H65" s="8"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
     </row>
     <row r="66" spans="1:8">
       <c r="B66" s="1"/>
-      <c r="G66" s="8"/>
-      <c r="H66" s="8"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
     </row>
     <row r="67" spans="1:8">
       <c r="B67" s="1"/>
-      <c r="G67" s="8"/>
-      <c r="H67" s="8"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
     </row>
     <row r="68" spans="1:8">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
-      <c r="G68" s="8"/>
-      <c r="H68" s="8"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
     </row>
     <row r="69" spans="1:8">
       <c r="B69" s="2"/>
@@ -2978,10 +2997,10 @@
       <c r="E70" t="s">
         <v>3</v>
       </c>
-      <c r="G70" s="8" t="s">
+      <c r="G70" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H70" s="8"/>
+      <c r="H70" s="6"/>
     </row>
     <row r="71" spans="1:8">
       <c r="A71">
@@ -2993,53 +3012,53 @@
       <c r="E71">
         <v>0.95000000079472802</v>
       </c>
-      <c r="G71" s="8"/>
-      <c r="H71" s="8"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
     </row>
     <row r="72" spans="1:8">
-      <c r="G72" s="8"/>
-      <c r="H72" s="8"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
     </row>
     <row r="73" spans="1:8">
-      <c r="G73" s="8"/>
-      <c r="H73" s="8"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
     </row>
     <row r="74" spans="1:8">
-      <c r="G74" s="8"/>
-      <c r="H74" s="8"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
     </row>
     <row r="75" spans="1:8">
-      <c r="G75" s="8"/>
-      <c r="H75" s="8"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
     </row>
     <row r="76" spans="1:8">
       <c r="B76" s="1"/>
-      <c r="G76" s="8"/>
-      <c r="H76" s="8"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
     </row>
     <row r="77" spans="1:8">
-      <c r="G77" s="8"/>
-      <c r="H77" s="8"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
     </row>
     <row r="78" spans="1:8">
-      <c r="G78" s="8"/>
-      <c r="H78" s="8"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
     </row>
     <row r="79" spans="1:8">
-      <c r="G79" s="8"/>
-      <c r="H79" s="8"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
     </row>
     <row r="80" spans="1:8">
-      <c r="G80" s="8"/>
-      <c r="H80" s="8"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
     </row>
     <row r="81" spans="1:8">
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
-      <c r="G81" s="8"/>
-      <c r="H81" s="8"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
     </row>
     <row r="82" spans="1:8">
       <c r="B82" s="2"/>
@@ -3073,10 +3092,10 @@
       <c r="E84" t="s">
         <v>3</v>
       </c>
-      <c r="G84" s="8" t="s">
+      <c r="G84" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H84" s="8"/>
+      <c r="H84" s="6"/>
     </row>
     <row r="85" spans="1:8">
       <c r="A85">
@@ -3089,61 +3108,61 @@
       <c r="E85">
         <v>0.94</v>
       </c>
-      <c r="G85" s="8"/>
-      <c r="H85" s="8"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
     </row>
     <row r="86" spans="1:8">
       <c r="B86" s="1"/>
-      <c r="G86" s="8"/>
-      <c r="H86" s="8"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
     </row>
     <row r="87" spans="1:8">
       <c r="B87" s="1"/>
-      <c r="G87" s="8"/>
-      <c r="H87" s="8"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
     </row>
     <row r="88" spans="1:8">
       <c r="B88" s="1"/>
-      <c r="G88" s="8"/>
-      <c r="H88" s="8"/>
+      <c r="G88" s="6"/>
+      <c r="H88" s="6"/>
     </row>
     <row r="89" spans="1:8">
       <c r="B89" s="1"/>
-      <c r="G89" s="8"/>
-      <c r="H89" s="8"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="6"/>
     </row>
     <row r="90" spans="1:8">
       <c r="B90" s="1"/>
-      <c r="G90" s="8"/>
-      <c r="H90" s="8"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
     </row>
     <row r="91" spans="1:8">
       <c r="B91" s="1"/>
-      <c r="G91" s="8"/>
-      <c r="H91" s="8"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="6"/>
     </row>
     <row r="92" spans="1:8">
       <c r="B92" s="1"/>
-      <c r="G92" s="8"/>
-      <c r="H92" s="8"/>
+      <c r="G92" s="6"/>
+      <c r="H92" s="6"/>
     </row>
     <row r="93" spans="1:8">
       <c r="B93" s="1"/>
-      <c r="G93" s="8"/>
-      <c r="H93" s="8"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
     </row>
     <row r="94" spans="1:8">
       <c r="B94" s="1"/>
-      <c r="G94" s="8"/>
-      <c r="H94" s="8"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="6"/>
     </row>
     <row r="95" spans="1:8">
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
-      <c r="G95" s="8"/>
-      <c r="H95" s="8"/>
+      <c r="G95" s="6"/>
+      <c r="H95" s="6"/>
     </row>
     <row r="96" spans="1:8">
       <c r="B96" s="2"/>
@@ -3169,10 +3188,10 @@
       <c r="E97" t="s">
         <v>3</v>
       </c>
-      <c r="G97" s="8" t="s">
+      <c r="G97" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H97" s="8"/>
+      <c r="H97" s="6"/>
     </row>
     <row r="98" spans="1:8">
       <c r="A98">
@@ -3184,52 +3203,52 @@
       <c r="E98">
         <v>0.94333333412806197</v>
       </c>
-      <c r="G98" s="8"/>
-      <c r="H98" s="8"/>
+      <c r="G98" s="6"/>
+      <c r="H98" s="6"/>
     </row>
     <row r="99" spans="1:8">
-      <c r="G99" s="8"/>
-      <c r="H99" s="8"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
     </row>
     <row r="100" spans="1:8">
-      <c r="G100" s="8"/>
-      <c r="H100" s="8"/>
+      <c r="G100" s="6"/>
+      <c r="H100" s="6"/>
     </row>
     <row r="101" spans="1:8">
-      <c r="G101" s="8"/>
-      <c r="H101" s="8"/>
+      <c r="G101" s="6"/>
+      <c r="H101" s="6"/>
     </row>
     <row r="102" spans="1:8">
-      <c r="G102" s="8"/>
-      <c r="H102" s="8"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
     </row>
     <row r="103" spans="1:8">
-      <c r="G103" s="8"/>
-      <c r="H103" s="8"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="6"/>
     </row>
     <row r="104" spans="1:8">
-      <c r="G104" s="8"/>
-      <c r="H104" s="8"/>
+      <c r="G104" s="6"/>
+      <c r="H104" s="6"/>
     </row>
     <row r="105" spans="1:8">
-      <c r="G105" s="8"/>
-      <c r="H105" s="8"/>
+      <c r="G105" s="6"/>
+      <c r="H105" s="6"/>
     </row>
     <row r="106" spans="1:8">
-      <c r="G106" s="8"/>
-      <c r="H106" s="8"/>
+      <c r="G106" s="6"/>
+      <c r="H106" s="6"/>
     </row>
     <row r="107" spans="1:8">
-      <c r="G107" s="8"/>
-      <c r="H107" s="8"/>
+      <c r="G107" s="6"/>
+      <c r="H107" s="6"/>
     </row>
     <row r="108" spans="1:8">
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
-      <c r="G108" s="8"/>
-      <c r="H108" s="8"/>
+      <c r="G108" s="6"/>
+      <c r="H108" s="6"/>
     </row>
     <row r="109" spans="1:8">
       <c r="B109" s="2"/>
@@ -3255,10 +3274,10 @@
       <c r="E110" t="s">
         <v>3</v>
       </c>
-      <c r="G110" s="8" t="s">
+      <c r="G110" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H110" s="8"/>
+      <c r="H110" s="10"/>
     </row>
     <row r="111" spans="1:8">
       <c r="A111">
@@ -3270,52 +3289,52 @@
       <c r="E111">
         <v>0.94333333333333302</v>
       </c>
-      <c r="G111" s="8"/>
-      <c r="H111" s="8"/>
+      <c r="G111" s="10"/>
+      <c r="H111" s="10"/>
     </row>
     <row r="112" spans="1:8">
-      <c r="G112" s="8"/>
-      <c r="H112" s="8"/>
+      <c r="G112" s="10"/>
+      <c r="H112" s="10"/>
     </row>
     <row r="113" spans="1:8">
-      <c r="G113" s="8"/>
-      <c r="H113" s="8"/>
+      <c r="G113" s="10"/>
+      <c r="H113" s="10"/>
     </row>
     <row r="114" spans="1:8">
-      <c r="G114" s="8"/>
-      <c r="H114" s="8"/>
+      <c r="G114" s="10"/>
+      <c r="H114" s="10"/>
     </row>
     <row r="115" spans="1:8">
-      <c r="G115" s="8"/>
-      <c r="H115" s="8"/>
+      <c r="G115" s="10"/>
+      <c r="H115" s="10"/>
     </row>
     <row r="116" spans="1:8">
-      <c r="G116" s="8"/>
-      <c r="H116" s="8"/>
+      <c r="G116" s="10"/>
+      <c r="H116" s="10"/>
     </row>
     <row r="117" spans="1:8">
-      <c r="G117" s="8"/>
-      <c r="H117" s="8"/>
+      <c r="G117" s="10"/>
+      <c r="H117" s="10"/>
     </row>
     <row r="118" spans="1:8">
-      <c r="G118" s="8"/>
-      <c r="H118" s="8"/>
+      <c r="G118" s="10"/>
+      <c r="H118" s="10"/>
     </row>
     <row r="119" spans="1:8">
-      <c r="G119" s="8"/>
-      <c r="H119" s="8"/>
+      <c r="G119" s="10"/>
+      <c r="H119" s="10"/>
     </row>
     <row r="120" spans="1:8">
-      <c r="G120" s="8"/>
-      <c r="H120" s="8"/>
+      <c r="G120" s="10"/>
+      <c r="H120" s="10"/>
     </row>
     <row r="121" spans="1:8">
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
-      <c r="G121" s="8"/>
-      <c r="H121" s="8"/>
+      <c r="G121" s="10"/>
+      <c r="H121" s="10"/>
     </row>
     <row r="122" spans="1:8">
       <c r="B122" s="2"/>
@@ -3365,10 +3384,10 @@
       <c r="E126" t="s">
         <v>3</v>
       </c>
-      <c r="G126" s="8" t="s">
+      <c r="G126" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H126" s="8"/>
+      <c r="H126" s="6"/>
     </row>
     <row r="127" spans="1:8">
       <c r="A127">
@@ -3380,53 +3399,53 @@
       <c r="E127">
         <v>0.49333333333333301</v>
       </c>
-      <c r="G127" s="8"/>
-      <c r="H127" s="8"/>
+      <c r="G127" s="6"/>
+      <c r="H127" s="6"/>
     </row>
     <row r="128" spans="1:8">
-      <c r="G128" s="8"/>
-      <c r="H128" s="8"/>
+      <c r="G128" s="6"/>
+      <c r="H128" s="6"/>
     </row>
     <row r="129" spans="1:8">
-      <c r="G129" s="8"/>
-      <c r="H129" s="8"/>
+      <c r="G129" s="6"/>
+      <c r="H129" s="6"/>
     </row>
     <row r="130" spans="1:8">
-      <c r="G130" s="8"/>
-      <c r="H130" s="8"/>
+      <c r="G130" s="6"/>
+      <c r="H130" s="6"/>
     </row>
     <row r="131" spans="1:8">
-      <c r="G131" s="8"/>
-      <c r="H131" s="8"/>
+      <c r="G131" s="6"/>
+      <c r="H131" s="6"/>
     </row>
     <row r="132" spans="1:8">
-      <c r="G132" s="8"/>
-      <c r="H132" s="8"/>
+      <c r="G132" s="6"/>
+      <c r="H132" s="6"/>
     </row>
     <row r="133" spans="1:8">
       <c r="B133" s="1"/>
-      <c r="G133" s="8"/>
-      <c r="H133" s="8"/>
+      <c r="G133" s="6"/>
+      <c r="H133" s="6"/>
     </row>
     <row r="134" spans="1:8">
-      <c r="G134" s="8"/>
-      <c r="H134" s="8"/>
+      <c r="G134" s="6"/>
+      <c r="H134" s="6"/>
     </row>
     <row r="135" spans="1:8">
-      <c r="G135" s="8"/>
-      <c r="H135" s="8"/>
+      <c r="G135" s="6"/>
+      <c r="H135" s="6"/>
     </row>
     <row r="136" spans="1:8">
-      <c r="G136" s="8"/>
-      <c r="H136" s="8"/>
+      <c r="G136" s="6"/>
+      <c r="H136" s="6"/>
     </row>
     <row r="137" spans="1:8">
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
       <c r="D137" s="2"/>
       <c r="E137" s="2"/>
-      <c r="G137" s="8"/>
-      <c r="H137" s="8"/>
+      <c r="G137" s="6"/>
+      <c r="H137" s="6"/>
     </row>
     <row r="138" spans="1:8">
       <c r="B138" s="2"/>
@@ -3450,10 +3469,10 @@
       <c r="E139" t="s">
         <v>3</v>
       </c>
-      <c r="G139" s="8" t="s">
+      <c r="G139" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H139" s="8"/>
+      <c r="H139" s="6"/>
     </row>
     <row r="140" spans="1:8">
       <c r="A140">
@@ -3465,53 +3484,53 @@
       <c r="E140">
         <v>0.94666666587193005</v>
       </c>
-      <c r="G140" s="8"/>
-      <c r="H140" s="8"/>
+      <c r="G140" s="6"/>
+      <c r="H140" s="6"/>
     </row>
     <row r="141" spans="1:8">
-      <c r="G141" s="8"/>
-      <c r="H141" s="8"/>
+      <c r="G141" s="6"/>
+      <c r="H141" s="6"/>
     </row>
     <row r="142" spans="1:8">
-      <c r="G142" s="8"/>
-      <c r="H142" s="8"/>
+      <c r="G142" s="6"/>
+      <c r="H142" s="6"/>
     </row>
     <row r="143" spans="1:8">
-      <c r="G143" s="8"/>
-      <c r="H143" s="8"/>
+      <c r="G143" s="6"/>
+      <c r="H143" s="6"/>
     </row>
     <row r="144" spans="1:8">
-      <c r="G144" s="8"/>
-      <c r="H144" s="8"/>
+      <c r="G144" s="6"/>
+      <c r="H144" s="6"/>
     </row>
     <row r="145" spans="1:8">
-      <c r="G145" s="8"/>
-      <c r="H145" s="8"/>
+      <c r="G145" s="6"/>
+      <c r="H145" s="6"/>
     </row>
     <row r="146" spans="1:8">
       <c r="B146" s="1"/>
-      <c r="G146" s="8"/>
-      <c r="H146" s="8"/>
+      <c r="G146" s="6"/>
+      <c r="H146" s="6"/>
     </row>
     <row r="147" spans="1:8">
-      <c r="G147" s="8"/>
-      <c r="H147" s="8"/>
+      <c r="G147" s="6"/>
+      <c r="H147" s="6"/>
     </row>
     <row r="148" spans="1:8">
-      <c r="G148" s="8"/>
-      <c r="H148" s="8"/>
+      <c r="G148" s="6"/>
+      <c r="H148" s="6"/>
     </row>
     <row r="149" spans="1:8">
-      <c r="G149" s="8"/>
-      <c r="H149" s="8"/>
+      <c r="G149" s="6"/>
+      <c r="H149" s="6"/>
     </row>
     <row r="150" spans="1:8">
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
       <c r="D150" s="2"/>
       <c r="E150" s="2"/>
-      <c r="G150" s="8"/>
-      <c r="H150" s="8"/>
+      <c r="G150" s="6"/>
+      <c r="H150" s="6"/>
     </row>
     <row r="151" spans="1:8">
       <c r="B151" s="2"/>
@@ -3535,10 +3554,10 @@
       <c r="E152" t="s">
         <v>3</v>
       </c>
-      <c r="G152" s="8" t="s">
+      <c r="G152" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H152" s="8"/>
+      <c r="H152" s="6"/>
     </row>
     <row r="153" spans="1:8">
       <c r="A153">
@@ -3550,53 +3569,53 @@
       <c r="E153">
         <v>0.93999999920520005</v>
       </c>
-      <c r="G153" s="8"/>
-      <c r="H153" s="8"/>
+      <c r="G153" s="6"/>
+      <c r="H153" s="6"/>
     </row>
     <row r="154" spans="1:8">
-      <c r="G154" s="8"/>
-      <c r="H154" s="8"/>
+      <c r="G154" s="6"/>
+      <c r="H154" s="6"/>
     </row>
     <row r="155" spans="1:8">
-      <c r="G155" s="8"/>
-      <c r="H155" s="8"/>
+      <c r="G155" s="6"/>
+      <c r="H155" s="6"/>
     </row>
     <row r="156" spans="1:8">
-      <c r="G156" s="8"/>
-      <c r="H156" s="8"/>
+      <c r="G156" s="6"/>
+      <c r="H156" s="6"/>
     </row>
     <row r="157" spans="1:8">
-      <c r="G157" s="8"/>
-      <c r="H157" s="8"/>
+      <c r="G157" s="6"/>
+      <c r="H157" s="6"/>
     </row>
     <row r="158" spans="1:8">
-      <c r="G158" s="8"/>
-      <c r="H158" s="8"/>
+      <c r="G158" s="6"/>
+      <c r="H158" s="6"/>
     </row>
     <row r="159" spans="1:8">
       <c r="B159" s="1"/>
-      <c r="G159" s="8"/>
-      <c r="H159" s="8"/>
+      <c r="G159" s="6"/>
+      <c r="H159" s="6"/>
     </row>
     <row r="160" spans="1:8">
-      <c r="G160" s="8"/>
-      <c r="H160" s="8"/>
+      <c r="G160" s="6"/>
+      <c r="H160" s="6"/>
     </row>
     <row r="161" spans="1:8">
-      <c r="G161" s="8"/>
-      <c r="H161" s="8"/>
+      <c r="G161" s="6"/>
+      <c r="H161" s="6"/>
     </row>
     <row r="162" spans="1:8">
-      <c r="G162" s="8"/>
-      <c r="H162" s="8"/>
+      <c r="G162" s="6"/>
+      <c r="H162" s="6"/>
     </row>
     <row r="163" spans="1:8">
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
       <c r="D163" s="2"/>
       <c r="E163" s="2"/>
-      <c r="G163" s="8"/>
-      <c r="H163" s="8"/>
+      <c r="G163" s="6"/>
+      <c r="H163" s="6"/>
     </row>
     <row r="164" spans="1:8">
       <c r="B164" s="2"/>
@@ -3620,62 +3639,62 @@
       <c r="E165" t="s">
         <v>3</v>
       </c>
-      <c r="G165" s="8" t="s">
+      <c r="G165" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H165" s="8"/>
+      <c r="H165" s="6"/>
     </row>
     <row r="166" spans="1:8">
       <c r="A166">
         <v>1</v>
       </c>
-      <c r="G166" s="8"/>
-      <c r="H166" s="8"/>
+      <c r="G166" s="6"/>
+      <c r="H166" s="6"/>
     </row>
     <row r="167" spans="1:8">
-      <c r="G167" s="8"/>
-      <c r="H167" s="8"/>
+      <c r="G167" s="6"/>
+      <c r="H167" s="6"/>
     </row>
     <row r="168" spans="1:8">
-      <c r="G168" s="8"/>
-      <c r="H168" s="8"/>
+      <c r="G168" s="6"/>
+      <c r="H168" s="6"/>
     </row>
     <row r="169" spans="1:8">
-      <c r="G169" s="8"/>
-      <c r="H169" s="8"/>
+      <c r="G169" s="6"/>
+      <c r="H169" s="6"/>
     </row>
     <row r="170" spans="1:8">
-      <c r="G170" s="8"/>
-      <c r="H170" s="8"/>
+      <c r="G170" s="6"/>
+      <c r="H170" s="6"/>
     </row>
     <row r="171" spans="1:8">
-      <c r="G171" s="8"/>
-      <c r="H171" s="8"/>
+      <c r="G171" s="6"/>
+      <c r="H171" s="6"/>
     </row>
     <row r="172" spans="1:8">
       <c r="B172" s="1"/>
-      <c r="G172" s="8"/>
-      <c r="H172" s="8"/>
+      <c r="G172" s="6"/>
+      <c r="H172" s="6"/>
     </row>
     <row r="173" spans="1:8">
-      <c r="G173" s="8"/>
-      <c r="H173" s="8"/>
+      <c r="G173" s="6"/>
+      <c r="H173" s="6"/>
     </row>
     <row r="174" spans="1:8">
-      <c r="G174" s="8"/>
-      <c r="H174" s="8"/>
+      <c r="G174" s="6"/>
+      <c r="H174" s="6"/>
     </row>
     <row r="175" spans="1:8">
-      <c r="G175" s="8"/>
-      <c r="H175" s="8"/>
+      <c r="G175" s="6"/>
+      <c r="H175" s="6"/>
     </row>
     <row r="176" spans="1:8">
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
       <c r="D176" s="2"/>
       <c r="E176" s="2"/>
-      <c r="G176" s="8"/>
-      <c r="H176" s="8"/>
+      <c r="G176" s="6"/>
+      <c r="H176" s="6"/>
     </row>
     <row r="177" spans="1:8">
       <c r="B177" s="2"/>
@@ -3699,10 +3718,10 @@
       <c r="E178" t="s">
         <v>3</v>
       </c>
-      <c r="G178" s="8" t="s">
+      <c r="G178" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H178" s="8"/>
+      <c r="H178" s="6"/>
     </row>
     <row r="179" spans="1:8">
       <c r="A179">
@@ -3714,53 +3733,53 @@
       <c r="E179">
         <v>0.93333333409999997</v>
       </c>
-      <c r="G179" s="8"/>
-      <c r="H179" s="8"/>
+      <c r="G179" s="6"/>
+      <c r="H179" s="6"/>
     </row>
     <row r="180" spans="1:8">
-      <c r="G180" s="8"/>
-      <c r="H180" s="8"/>
+      <c r="G180" s="6"/>
+      <c r="H180" s="6"/>
     </row>
     <row r="181" spans="1:8">
-      <c r="G181" s="8"/>
-      <c r="H181" s="8"/>
+      <c r="G181" s="6"/>
+      <c r="H181" s="6"/>
     </row>
     <row r="182" spans="1:8">
-      <c r="G182" s="8"/>
-      <c r="H182" s="8"/>
+      <c r="G182" s="6"/>
+      <c r="H182" s="6"/>
     </row>
     <row r="183" spans="1:8">
-      <c r="G183" s="8"/>
-      <c r="H183" s="8"/>
+      <c r="G183" s="6"/>
+      <c r="H183" s="6"/>
     </row>
     <row r="184" spans="1:8">
-      <c r="G184" s="8"/>
-      <c r="H184" s="8"/>
+      <c r="G184" s="6"/>
+      <c r="H184" s="6"/>
     </row>
     <row r="185" spans="1:8">
       <c r="B185" s="1"/>
-      <c r="G185" s="8"/>
-      <c r="H185" s="8"/>
+      <c r="G185" s="6"/>
+      <c r="H185" s="6"/>
     </row>
     <row r="186" spans="1:8">
-      <c r="G186" s="8"/>
-      <c r="H186" s="8"/>
+      <c r="G186" s="6"/>
+      <c r="H186" s="6"/>
     </row>
     <row r="187" spans="1:8">
-      <c r="G187" s="8"/>
-      <c r="H187" s="8"/>
+      <c r="G187" s="6"/>
+      <c r="H187" s="6"/>
     </row>
     <row r="188" spans="1:8">
-      <c r="G188" s="8"/>
-      <c r="H188" s="8"/>
+      <c r="G188" s="6"/>
+      <c r="H188" s="6"/>
     </row>
     <row r="189" spans="1:8">
       <c r="B189" s="2"/>
       <c r="C189" s="2"/>
       <c r="D189" s="2"/>
       <c r="E189" s="2"/>
-      <c r="G189" s="8"/>
-      <c r="H189" s="8"/>
+      <c r="G189" s="6"/>
+      <c r="H189" s="6"/>
     </row>
     <row r="191" spans="1:8">
       <c r="A191" t="s">
@@ -3783,8 +3802,8 @@
       <c r="C192">
         <v>0.95</v>
       </c>
-      <c r="G192" s="8"/>
-      <c r="H192" s="8"/>
+      <c r="G192" s="6"/>
+      <c r="H192" s="6"/>
     </row>
     <row r="193" spans="1:8">
       <c r="A193">
@@ -3796,8 +3815,8 @@
       <c r="C193">
         <v>0.93</v>
       </c>
-      <c r="G193" s="8"/>
-      <c r="H193" s="8"/>
+      <c r="G193" s="6"/>
+      <c r="H193" s="6"/>
     </row>
     <row r="194" spans="1:8">
       <c r="A194">
@@ -3809,8 +3828,8 @@
       <c r="C194">
         <v>0.93330000000000002</v>
       </c>
-      <c r="G194" s="8"/>
-      <c r="H194" s="8"/>
+      <c r="G194" s="6"/>
+      <c r="H194" s="6"/>
     </row>
     <row r="195" spans="1:8">
       <c r="A195">
@@ -3822,8 +3841,8 @@
       <c r="C195">
         <v>0.88</v>
       </c>
-      <c r="G195" s="8"/>
-      <c r="H195" s="8"/>
+      <c r="G195" s="6"/>
+      <c r="H195" s="6"/>
     </row>
     <row r="196" spans="1:8">
       <c r="A196">
@@ -3835,12 +3854,12 @@
       <c r="C196">
         <v>0.49330000000000002</v>
       </c>
-      <c r="G196" s="8"/>
-      <c r="H196" s="8"/>
+      <c r="G196" s="6"/>
+      <c r="H196" s="6"/>
     </row>
     <row r="197" spans="1:8">
-      <c r="G197" s="8"/>
-      <c r="H197" s="8"/>
+      <c r="G197" s="6"/>
+      <c r="H197" s="6"/>
     </row>
     <row r="198" spans="1:8">
       <c r="A198" t="s">
@@ -3849,8 +3868,8 @@
       <c r="B198" t="s">
         <v>27</v>
       </c>
-      <c r="G198" s="8"/>
-      <c r="H198" s="8"/>
+      <c r="G198" s="6"/>
+      <c r="H198" s="6"/>
     </row>
     <row r="199" spans="1:8">
       <c r="A199">
@@ -3859,8 +3878,8 @@
       <c r="B199">
         <v>0.49330000000000002</v>
       </c>
-      <c r="G199" s="8"/>
-      <c r="H199" s="8"/>
+      <c r="G199" s="6"/>
+      <c r="H199" s="6"/>
     </row>
     <row r="200" spans="1:8">
       <c r="A200">
@@ -3869,8 +3888,8 @@
       <c r="B200">
         <v>0.88</v>
       </c>
-      <c r="G200" s="8"/>
-      <c r="H200" s="8"/>
+      <c r="G200" s="6"/>
+      <c r="H200" s="6"/>
     </row>
     <row r="201" spans="1:8">
       <c r="A201">
@@ -3879,8 +3898,8 @@
       <c r="B201">
         <v>0.93330000000000002</v>
       </c>
-      <c r="G201" s="8"/>
-      <c r="H201" s="8"/>
+      <c r="G201" s="6"/>
+      <c r="H201" s="6"/>
     </row>
     <row r="202" spans="1:8">
       <c r="A202">
@@ -3889,8 +3908,8 @@
       <c r="B202">
         <v>0.93</v>
       </c>
-      <c r="G202" s="8"/>
-      <c r="H202" s="8"/>
+      <c r="G202" s="6"/>
+      <c r="H202" s="6"/>
     </row>
     <row r="203" spans="1:8">
       <c r="A203">
@@ -3902,80 +3921,80 @@
       <c r="C203" s="2"/>
       <c r="D203" s="2"/>
       <c r="E203" s="2"/>
-      <c r="G203" s="8"/>
-      <c r="H203" s="8"/>
+      <c r="G203" s="6"/>
+      <c r="H203" s="6"/>
     </row>
     <row r="205" spans="1:8">
-      <c r="G205" s="8"/>
-      <c r="H205" s="8"/>
+      <c r="G205" s="6"/>
+      <c r="H205" s="6"/>
     </row>
     <row r="206" spans="1:8">
-      <c r="G206" s="8"/>
-      <c r="H206" s="8"/>
+      <c r="G206" s="6"/>
+      <c r="H206" s="6"/>
     </row>
     <row r="207" spans="1:8">
-      <c r="G207" s="8"/>
-      <c r="H207" s="8"/>
+      <c r="G207" s="6"/>
+      <c r="H207" s="6"/>
     </row>
     <row r="208" spans="1:8">
-      <c r="G208" s="8"/>
-      <c r="H208" s="8"/>
+      <c r="G208" s="6"/>
+      <c r="H208" s="6"/>
     </row>
     <row r="209" spans="2:8">
-      <c r="G209" s="8"/>
-      <c r="H209" s="8"/>
+      <c r="G209" s="6"/>
+      <c r="H209" s="6"/>
     </row>
     <row r="210" spans="2:8">
-      <c r="G210" s="8"/>
-      <c r="H210" s="8"/>
+      <c r="G210" s="6"/>
+      <c r="H210" s="6"/>
     </row>
     <row r="211" spans="2:8">
-      <c r="G211" s="8"/>
-      <c r="H211" s="8"/>
+      <c r="G211" s="6"/>
+      <c r="H211" s="6"/>
     </row>
     <row r="212" spans="2:8">
       <c r="B212" s="1"/>
-      <c r="G212" s="8"/>
-      <c r="H212" s="8"/>
+      <c r="G212" s="6"/>
+      <c r="H212" s="6"/>
     </row>
     <row r="213" spans="2:8">
-      <c r="G213" s="8"/>
-      <c r="H213" s="8"/>
+      <c r="G213" s="6"/>
+      <c r="H213" s="6"/>
     </row>
     <row r="214" spans="2:8">
-      <c r="G214" s="8"/>
-      <c r="H214" s="8"/>
+      <c r="G214" s="6"/>
+      <c r="H214" s="6"/>
     </row>
     <row r="215" spans="2:8">
-      <c r="G215" s="8"/>
-      <c r="H215" s="8"/>
+      <c r="G215" s="6"/>
+      <c r="H215" s="6"/>
     </row>
     <row r="216" spans="2:8">
       <c r="B216" s="2"/>
       <c r="C216" s="2"/>
       <c r="D216" s="2"/>
       <c r="E216" s="2"/>
-      <c r="G216" s="8"/>
-      <c r="H216" s="8"/>
+      <c r="G216" s="6"/>
+      <c r="H216" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="G1:H12"/>
+    <mergeCell ref="G16:H26"/>
+    <mergeCell ref="G29:H39"/>
+    <mergeCell ref="G42:H52"/>
+    <mergeCell ref="G57:H68"/>
+    <mergeCell ref="G70:H81"/>
+    <mergeCell ref="G84:H95"/>
+    <mergeCell ref="G97:H108"/>
+    <mergeCell ref="G110:H121"/>
+    <mergeCell ref="G126:H137"/>
     <mergeCell ref="G205:H216"/>
     <mergeCell ref="G139:H150"/>
     <mergeCell ref="G152:H163"/>
     <mergeCell ref="G165:H176"/>
     <mergeCell ref="G178:H189"/>
     <mergeCell ref="G192:H203"/>
-    <mergeCell ref="G70:H81"/>
-    <mergeCell ref="G84:H95"/>
-    <mergeCell ref="G97:H108"/>
-    <mergeCell ref="G110:H121"/>
-    <mergeCell ref="G126:H137"/>
-    <mergeCell ref="G1:H12"/>
-    <mergeCell ref="G16:H26"/>
-    <mergeCell ref="G29:H39"/>
-    <mergeCell ref="G42:H52"/>
-    <mergeCell ref="G57:H68"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>